<commit_message>
ejercicio 5 arreglado plots de 5,6,7. Los plots del 6 estn mal
</commit_message>
<xml_diff>
--- a/plots/plots-ej4/resumen_lambda.xlsx
+++ b/plots/plots-ej4/resumen_lambda.xlsx
@@ -505,41 +505,41 @@
         <v>0.02</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1205555555555556</v>
+        <v>0.1002355555555555</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00767470280207235</v>
+        <v>0.000316558558665647</v>
       </c>
       <c r="D2" t="n">
-        <v>1800</v>
+        <v>900000</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1133302368787738</v>
+        <v>0.0952617871626035</v>
       </c>
       <c r="F2" t="n">
-        <v>0.006831747910401472</v>
+        <v>0.0002825813553880523</v>
       </c>
       <c r="G2" t="n">
-        <v>2153</v>
+        <v>1079331</v>
       </c>
       <c r="H2" t="n">
-        <v>0.04226660473757548</v>
+        <v>0.01595803326319729</v>
       </c>
       <c r="I2" t="n">
-        <v>0.004336096929523857</v>
+        <v>0.0001206199565628483</v>
       </c>
       <c r="J2" t="n">
-        <v>2153</v>
+        <v>1079331</v>
       </c>
       <c r="K2" t="n">
-        <v>0.03121588248797468</v>
+        <v>0.01132876132421023</v>
       </c>
       <c r="L2" t="n">
-        <v>0.006151535709242239</v>
+        <v>8.13425463776297e-05</v>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>run_p=0.02_sim=100.json</t>
+          <t>run_p=0.02_sim=50000.json</t>
         </is>
       </c>
     </row>
@@ -548,41 +548,41 @@
         <v>0.1</v>
       </c>
       <c r="B3" t="n">
-        <v>0.8511111111111112</v>
+        <v>0.8521133333333333</v>
       </c>
       <c r="C3" t="n">
-        <v>0.008390503482917158</v>
+        <v>0.0003741897921419155</v>
       </c>
       <c r="D3" t="n">
-        <v>1800</v>
+        <v>900000</v>
       </c>
       <c r="E3" t="n">
-        <v>0.4231447942788149</v>
+        <v>0.4019729960584148</v>
       </c>
       <c r="F3" t="n">
-        <v>0.004761354886784242</v>
+        <v>0.000210977949417813</v>
       </c>
       <c r="G3" t="n">
-        <v>10767</v>
+        <v>5400619</v>
       </c>
       <c r="H3" t="n">
-        <v>0.128726664809139</v>
+        <v>0.05253453354143293</v>
       </c>
       <c r="I3" t="n">
-        <v>0.00322748411576164</v>
+        <v>9.600246074253525e-05</v>
       </c>
       <c r="J3" t="n">
-        <v>10767</v>
+        <v>5400619</v>
       </c>
       <c r="K3" t="n">
-        <v>0.913289956167127</v>
+        <v>0.05824890767162477</v>
       </c>
       <c r="L3" t="n">
-        <v>0.05855463743844452</v>
+        <v>8.615328976067394e-05</v>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>run_p=0.1_sim=100.json</t>
+          <t>run_p=0.1_sim=50000.json</t>
         </is>
       </c>
     </row>
@@ -591,41 +591,41 @@
         <v>0.2</v>
       </c>
       <c r="B4" t="n">
-        <v>0.995</v>
+        <v>0.9973588888888889</v>
       </c>
       <c r="C4" t="n">
-        <v>0.001662494778605001</v>
+        <v>5.410006821940513e-05</v>
       </c>
       <c r="D4" t="n">
-        <v>1800</v>
+        <v>900000</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7704841277273153</v>
+        <v>0.6463261083130704</v>
       </c>
       <c r="F4" t="n">
-        <v>0.002877450885756958</v>
+        <v>0.0001454973372395505</v>
       </c>
       <c r="G4" t="n">
-        <v>21358</v>
+        <v>10798032</v>
       </c>
       <c r="H4" t="n">
-        <v>0.07374285981833505</v>
+        <v>0.1051356395313516</v>
       </c>
       <c r="I4" t="n">
-        <v>0.001788321020010896</v>
+        <v>9.334289822630437e-05</v>
       </c>
       <c r="J4" t="n">
-        <v>21358</v>
+        <v>10798032</v>
       </c>
       <c r="K4" t="n">
-        <v>6.240274223148208</v>
+        <v>0.1122863190711461</v>
       </c>
       <c r="L4" t="n">
-        <v>0.09561850562227824</v>
+        <v>8.987246824041488e-05</v>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>run_p=0.2_sim=100.json</t>
+          <t>run_p=0.2_sim=50000.json</t>
         </is>
       </c>
     </row>
@@ -640,35 +640,35 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1800</v>
+        <v>900000</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9862312412212612</v>
+        <v>0.9323585417411794</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0005009634404605257</v>
+        <v>4.83370582491058e-05</v>
       </c>
       <c r="G5" t="n">
-        <v>54108</v>
+        <v>26992026</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0003511495527463591</v>
+        <v>0.3403622240138625</v>
       </c>
       <c r="I5" t="n">
-        <v>8.054508693052461e-05</v>
+        <v>9.120227967027469e-05</v>
       </c>
       <c r="J5" t="n">
-        <v>54108</v>
+        <v>26992026</v>
       </c>
       <c r="K5" t="n">
-        <v>8.553737504064456</v>
+        <v>0.2702761783178307</v>
       </c>
       <c r="L5" t="n">
-        <v>0.01149978735899419</v>
+        <v>9.577233979532408e-05</v>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>run_p=0.5_sim=100.json</t>
+          <t>run_p=0.5_sim=50000.json</t>
         </is>
       </c>
     </row>
@@ -683,35 +683,35 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1800</v>
+        <v>900000</v>
       </c>
       <c r="E6" t="n">
-        <v>0.9990740740740741</v>
+        <v>0.9953703703703703</v>
       </c>
       <c r="F6" t="n">
-        <v>9.254971572407588e-05</v>
+        <v>9.237800923903298e-06</v>
       </c>
       <c r="G6" t="n">
-        <v>108000</v>
+        <v>54000000</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>0.575925925925926</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>6.725232389930653e-05</v>
       </c>
       <c r="J6" t="n">
-        <v>108000</v>
+        <v>54000000</v>
       </c>
       <c r="K6" t="n">
-        <v>8.592748091603061</v>
+        <v>0.5939393939393953</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>4.965117957922383e-19</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>run_p=1_sim=100.json</t>
+          <t>run_p=1_sim=50000.json</t>
         </is>
       </c>
     </row>

</xml_diff>